<commit_message>
Commit to test Jenkins trigger
</commit_message>
<xml_diff>
--- a/MavenProjectPOMThreadLocal/Data/cloneContactReq.xlsx
+++ b/MavenProjectPOMThreadLocal/Data/cloneContactReq.xlsx
@@ -30,10 +30,10 @@
     <t>9999888866</t>
   </si>
   <si>
-    <t>00000003</t>
-  </si>
-  <si>
-    <t>00000014</t>
+    <t>00000080</t>
+  </si>
+  <si>
+    <t>00000081</t>
   </si>
 </sst>
 </file>
@@ -369,7 +369,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>